<commit_message>
Reordering and Binding of Sensor logic.
</commit_message>
<xml_diff>
--- a/doc/BTI7301 SearchRobot Projektplan.xlsx
+++ b/doc/BTI7301 SearchRobot Projektplan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1460" windowWidth="26420" windowHeight="16500"/>
+    <workbookView xWindow="1260" yWindow="1455" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -163,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +179,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +271,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -280,6 +292,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,20 +303,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,121 +638,121 @@
   <dimension ref="A1:BM185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-    <col min="2" max="65" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="65" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-    </row>
-    <row r="2" spans="1:65">
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="18" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="18" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="19"/>
-      <c r="T2" s="19"/>
-      <c r="U2" s="19"/>
-      <c r="V2" s="19"/>
-      <c r="W2" s="19"/>
-      <c r="X2" s="19"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="18" t="s">
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="18" t="s">
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="AI2" s="19"/>
-      <c r="AJ2" s="19"/>
-      <c r="AK2" s="19"/>
-      <c r="AL2" s="19"/>
-      <c r="AM2" s="19"/>
-      <c r="AN2" s="19"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="18" t="s">
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="AQ2" s="19"/>
-      <c r="AR2" s="19"/>
-      <c r="AS2" s="19"/>
-      <c r="AT2" s="19"/>
-      <c r="AU2" s="19"/>
-      <c r="AV2" s="19"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="18" t="s">
+      <c r="AQ2" s="26"/>
+      <c r="AR2" s="26"/>
+      <c r="AS2" s="26"/>
+      <c r="AT2" s="26"/>
+      <c r="AU2" s="26"/>
+      <c r="AV2" s="26"/>
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="AY2" s="19"/>
-      <c r="AZ2" s="19"/>
-      <c r="BA2" s="19"/>
-      <c r="BB2" s="19"/>
-      <c r="BC2" s="19"/>
-      <c r="BD2" s="19"/>
-      <c r="BE2" s="20"/>
-      <c r="BF2" s="21"/>
-      <c r="BG2" s="21"/>
-      <c r="BH2" s="21"/>
-      <c r="BI2" s="21"/>
-      <c r="BJ2" s="21"/>
-      <c r="BK2" s="21"/>
-      <c r="BL2" s="21"/>
-      <c r="BM2" s="21"/>
-    </row>
-    <row r="3" spans="1:65">
+      <c r="AY2" s="26"/>
+      <c r="AZ2" s="26"/>
+      <c r="BA2" s="26"/>
+      <c r="BB2" s="26"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="26"/>
+      <c r="BE2" s="27"/>
+      <c r="BF2" s="24"/>
+      <c r="BG2" s="24"/>
+      <c r="BH2" s="24"/>
+      <c r="BI2" s="24"/>
+      <c r="BJ2" s="24"/>
+      <c r="BK2" s="24"/>
+      <c r="BL2" s="24"/>
+      <c r="BM2" s="24"/>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -783,7 +813,7 @@
       <c r="BD3" s="2"/>
       <c r="BE3" s="3"/>
     </row>
-    <row r="4" spans="1:65">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -844,7 +874,7 @@
       <c r="BD4" s="2"/>
       <c r="BE4" s="3"/>
     </row>
-    <row r="5" spans="1:65">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -905,7 +935,7 @@
       <c r="BD5" s="2"/>
       <c r="BE5" s="3"/>
     </row>
-    <row r="6" spans="1:65">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -929,10 +959,10 @@
       <c r="S6" s="16"/>
       <c r="T6" s="16"/>
       <c r="U6" s="16"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="24"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="19"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
@@ -966,7 +996,7 @@
       <c r="BD6" s="2"/>
       <c r="BE6" s="3"/>
     </row>
-    <row r="7" spans="1:65">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1027,7 +1057,7 @@
       <c r="BD7" s="2"/>
       <c r="BE7" s="3"/>
     </row>
-    <row r="8" spans="1:65">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1088,7 +1118,7 @@
       <c r="BD8" s="11"/>
       <c r="BE8" s="12"/>
     </row>
-    <row r="9" spans="1:65">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1149,7 +1179,7 @@
       <c r="BD9" s="8"/>
       <c r="BE9" s="9"/>
     </row>
-    <row r="10" spans="1:65">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1207,7 +1237,7 @@
       <c r="BD10" s="2"/>
       <c r="BE10" s="3"/>
     </row>
-    <row r="11" spans="1:65">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1265,7 +1295,7 @@
       <c r="BD11" s="2"/>
       <c r="BE11" s="3"/>
     </row>
-    <row r="12" spans="1:65">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1323,82 +1353,82 @@
       <c r="BD12" s="2"/>
       <c r="BE12" s="3"/>
     </row>
-    <row r="13" spans="1:65">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="18" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="18" t="s">
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="S13" s="19"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="18" t="s">
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
-      <c r="AC13" s="19"/>
-      <c r="AD13" s="19"/>
-      <c r="AE13" s="19"/>
-      <c r="AF13" s="19"/>
-      <c r="AG13" s="20"/>
-      <c r="AH13" s="18" t="s">
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="21"/>
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="21"/>
+      <c r="AG13" s="22"/>
+      <c r="AH13" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AI13" s="19"/>
-      <c r="AJ13" s="19"/>
-      <c r="AK13" s="19"/>
-      <c r="AL13" s="19"/>
-      <c r="AM13" s="19"/>
-      <c r="AN13" s="19"/>
-      <c r="AO13" s="20"/>
-      <c r="AP13" s="18" t="s">
+      <c r="AI13" s="21"/>
+      <c r="AJ13" s="21"/>
+      <c r="AK13" s="21"/>
+      <c r="AL13" s="21"/>
+      <c r="AM13" s="21"/>
+      <c r="AN13" s="21"/>
+      <c r="AO13" s="22"/>
+      <c r="AP13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="AQ13" s="19"/>
-      <c r="AR13" s="19"/>
-      <c r="AS13" s="19"/>
-      <c r="AT13" s="19"/>
-      <c r="AU13" s="19"/>
-      <c r="AV13" s="19"/>
-      <c r="AW13" s="20"/>
-      <c r="AX13" s="18" t="s">
+      <c r="AQ13" s="21"/>
+      <c r="AR13" s="21"/>
+      <c r="AS13" s="21"/>
+      <c r="AT13" s="21"/>
+      <c r="AU13" s="21"/>
+      <c r="AV13" s="21"/>
+      <c r="AW13" s="22"/>
+      <c r="AX13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="AY13" s="19"/>
-      <c r="AZ13" s="19"/>
-      <c r="BA13" s="19"/>
-      <c r="BB13" s="19"/>
-      <c r="BC13" s="19"/>
-      <c r="BD13" s="19"/>
-      <c r="BE13" s="20"/>
-    </row>
-    <row r="14" spans="1:65">
+      <c r="AY13" s="21"/>
+      <c r="AZ13" s="21"/>
+      <c r="BA13" s="21"/>
+      <c r="BB13" s="21"/>
+      <c r="BC13" s="21"/>
+      <c r="BD13" s="21"/>
+      <c r="BE13" s="22"/>
+    </row>
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1459,7 +1489,7 @@
       <c r="BD14" s="2"/>
       <c r="BE14" s="3"/>
     </row>
-    <row r="15" spans="1:65">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1520,7 +1550,7 @@
       <c r="BD15" s="2"/>
       <c r="BE15" s="3"/>
     </row>
-    <row r="16" spans="1:65">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1581,7 +1611,7 @@
       <c r="BD16" s="2"/>
       <c r="BE16" s="3"/>
     </row>
-    <row r="17" spans="1:60">
+    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1642,7 +1672,7 @@
       <c r="BD17" s="2"/>
       <c r="BE17" s="3"/>
     </row>
-    <row r="18" spans="1:60">
+    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1703,7 +1733,7 @@
       <c r="BD18" s="2"/>
       <c r="BE18" s="3"/>
     </row>
-    <row r="19" spans="1:60">
+    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1764,7 +1794,7 @@
       <c r="BD19" s="11"/>
       <c r="BE19" s="12"/>
     </row>
-    <row r="20" spans="1:60">
+    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1825,7 +1855,7 @@
       <c r="BD20" s="8"/>
       <c r="BE20" s="9"/>
     </row>
-    <row r="21" spans="1:60">
+    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1883,7 +1913,7 @@
       <c r="BD21" s="2"/>
       <c r="BE21" s="3"/>
     </row>
-    <row r="22" spans="1:60">
+    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1941,7 +1971,7 @@
       <c r="BD22" s="2"/>
       <c r="BE22" s="3"/>
     </row>
-    <row r="23" spans="1:60">
+    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1999,7 +2029,7 @@
       <c r="BD23" s="2"/>
       <c r="BE23" s="3"/>
     </row>
-    <row r="24" spans="1:60">
+    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2057,72 +2087,72 @@
       <c r="BD24" s="2"/>
       <c r="BE24" s="3"/>
     </row>
-    <row r="25" spans="1:60">
+    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="18" t="s">
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="19"/>
-      <c r="X25" s="19"/>
-      <c r="Y25" s="20"/>
-      <c r="Z25" s="18"/>
-      <c r="AA25" s="19"/>
-      <c r="AB25" s="19"/>
-      <c r="AC25" s="19"/>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="19"/>
-      <c r="AF25" s="19"/>
-      <c r="AG25" s="20"/>
-      <c r="AH25" s="18"/>
-      <c r="AI25" s="19"/>
-      <c r="AJ25" s="19"/>
-      <c r="AK25" s="19"/>
-      <c r="AL25" s="19"/>
-      <c r="AM25" s="19"/>
-      <c r="AN25" s="19"/>
-      <c r="AO25" s="20"/>
-      <c r="AP25" s="18"/>
-      <c r="AQ25" s="19"/>
-      <c r="AR25" s="19"/>
-      <c r="AS25" s="19"/>
-      <c r="AT25" s="19"/>
-      <c r="AU25" s="19"/>
-      <c r="AV25" s="19"/>
-      <c r="AW25" s="20"/>
-      <c r="AX25" s="18"/>
-      <c r="AY25" s="19"/>
-      <c r="AZ25" s="19"/>
-      <c r="BA25" s="19"/>
-      <c r="BB25" s="19"/>
-      <c r="BC25" s="19"/>
-      <c r="BD25" s="19"/>
-      <c r="BE25" s="20"/>
-    </row>
-    <row r="26" spans="1:60">
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="22"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="21"/>
+      <c r="AB25" s="21"/>
+      <c r="AC25" s="21"/>
+      <c r="AD25" s="21"/>
+      <c r="AE25" s="21"/>
+      <c r="AF25" s="21"/>
+      <c r="AG25" s="22"/>
+      <c r="AH25" s="20"/>
+      <c r="AI25" s="21"/>
+      <c r="AJ25" s="21"/>
+      <c r="AK25" s="21"/>
+      <c r="AL25" s="21"/>
+      <c r="AM25" s="21"/>
+      <c r="AN25" s="21"/>
+      <c r="AO25" s="22"/>
+      <c r="AP25" s="20"/>
+      <c r="AQ25" s="21"/>
+      <c r="AR25" s="21"/>
+      <c r="AS25" s="21"/>
+      <c r="AT25" s="21"/>
+      <c r="AU25" s="21"/>
+      <c r="AV25" s="21"/>
+      <c r="AW25" s="22"/>
+      <c r="AX25" s="20"/>
+      <c r="AY25" s="21"/>
+      <c r="AZ25" s="21"/>
+      <c r="BA25" s="21"/>
+      <c r="BB25" s="21"/>
+      <c r="BC25" s="21"/>
+      <c r="BD25" s="21"/>
+      <c r="BE25" s="22"/>
+    </row>
+    <row r="26" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2183,7 +2213,7 @@
       <c r="BD26" s="2"/>
       <c r="BE26" s="3"/>
     </row>
-    <row r="27" spans="1:60">
+    <row r="27" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -2244,7 +2274,7 @@
       <c r="BD27" s="2"/>
       <c r="BE27" s="3"/>
     </row>
-    <row r="28" spans="1:60">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2302,7 +2332,7 @@
       <c r="BD28" s="2"/>
       <c r="BE28" s="3"/>
     </row>
-    <row r="29" spans="1:60">
+    <row r="29" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2360,7 +2390,7 @@
       <c r="BD29" s="2"/>
       <c r="BE29" s="3"/>
     </row>
-    <row r="30" spans="1:60">
+    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2418,7 +2448,7 @@
       <c r="BD30" s="2"/>
       <c r="BE30" s="3"/>
     </row>
-    <row r="31" spans="1:60">
+    <row r="31" spans="1:60" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2476,7 +2506,7 @@
       <c r="BD31" s="2"/>
       <c r="BE31" s="3"/>
     </row>
-    <row r="32" spans="1:60">
+    <row r="32" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2538,7 +2568,7 @@
       <c r="BG32" s="2"/>
       <c r="BH32" s="2"/>
     </row>
-    <row r="33" spans="1:60">
+    <row r="33" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2600,7 +2630,7 @@
       <c r="BG33" s="2"/>
       <c r="BH33" s="2"/>
     </row>
-    <row r="34" spans="1:60">
+    <row r="34" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2662,7 +2692,7 @@
       <c r="BG34" s="2"/>
       <c r="BH34" s="2"/>
     </row>
-    <row r="35" spans="1:60">
+    <row r="35" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2724,7 +2754,7 @@
       <c r="BG35" s="2"/>
       <c r="BH35" s="2"/>
     </row>
-    <row r="36" spans="1:60">
+    <row r="36" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2786,7 +2816,7 @@
       <c r="BG36" s="2"/>
       <c r="BH36" s="2"/>
     </row>
-    <row r="37" spans="1:60">
+    <row r="37" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2848,7 +2878,7 @@
       <c r="BG37" s="2"/>
       <c r="BH37" s="2"/>
     </row>
-    <row r="38" spans="1:60">
+    <row r="38" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2910,7 +2940,7 @@
       <c r="BG38" s="2"/>
       <c r="BH38" s="2"/>
     </row>
-    <row r="39" spans="1:60">
+    <row r="39" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2972,7 +3002,7 @@
       <c r="BG39" s="2"/>
       <c r="BH39" s="2"/>
     </row>
-    <row r="40" spans="1:60">
+    <row r="40" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3034,7 +3064,7 @@
       <c r="BG40" s="2"/>
       <c r="BH40" s="2"/>
     </row>
-    <row r="41" spans="1:60">
+    <row r="41" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3096,7 +3126,7 @@
       <c r="BG41" s="2"/>
       <c r="BH41" s="2"/>
     </row>
-    <row r="42" spans="1:60">
+    <row r="42" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3158,7 +3188,7 @@
       <c r="BG42" s="2"/>
       <c r="BH42" s="2"/>
     </row>
-    <row r="43" spans="1:60">
+    <row r="43" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3220,7 +3250,7 @@
       <c r="BG43" s="2"/>
       <c r="BH43" s="2"/>
     </row>
-    <row r="44" spans="1:60">
+    <row r="44" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3282,7 +3312,7 @@
       <c r="BG44" s="2"/>
       <c r="BH44" s="2"/>
     </row>
-    <row r="45" spans="1:60">
+    <row r="45" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3344,7 +3374,7 @@
       <c r="BG45" s="2"/>
       <c r="BH45" s="2"/>
     </row>
-    <row r="46" spans="1:60">
+    <row r="46" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3406,7 +3436,7 @@
       <c r="BG46" s="2"/>
       <c r="BH46" s="2"/>
     </row>
-    <row r="47" spans="1:60">
+    <row r="47" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3468,7 +3498,7 @@
       <c r="BG47" s="2"/>
       <c r="BH47" s="2"/>
     </row>
-    <row r="48" spans="1:60">
+    <row r="48" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3530,7 +3560,7 @@
       <c r="BG48" s="2"/>
       <c r="BH48" s="2"/>
     </row>
-    <row r="49" spans="1:60">
+    <row r="49" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -3592,7 +3622,7 @@
       <c r="BG49" s="2"/>
       <c r="BH49" s="2"/>
     </row>
-    <row r="50" spans="1:60">
+    <row r="50" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -3654,7 +3684,7 @@
       <c r="BG50" s="2"/>
       <c r="BH50" s="2"/>
     </row>
-    <row r="51" spans="1:60">
+    <row r="51" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3716,7 +3746,7 @@
       <c r="BG51" s="2"/>
       <c r="BH51" s="2"/>
     </row>
-    <row r="52" spans="1:60">
+    <row r="52" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -3778,7 +3808,7 @@
       <c r="BG52" s="2"/>
       <c r="BH52" s="2"/>
     </row>
-    <row r="53" spans="1:60">
+    <row r="53" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -3840,7 +3870,7 @@
       <c r="BG53" s="2"/>
       <c r="BH53" s="2"/>
     </row>
-    <row r="54" spans="1:60">
+    <row r="54" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -3902,7 +3932,7 @@
       <c r="BG54" s="2"/>
       <c r="BH54" s="2"/>
     </row>
-    <row r="55" spans="1:60">
+    <row r="55" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -3964,7 +3994,7 @@
       <c r="BG55" s="2"/>
       <c r="BH55" s="2"/>
     </row>
-    <row r="56" spans="1:60">
+    <row r="56" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -4026,7 +4056,7 @@
       <c r="BG56" s="2"/>
       <c r="BH56" s="2"/>
     </row>
-    <row r="57" spans="1:60">
+    <row r="57" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -4088,7 +4118,7 @@
       <c r="BG57" s="2"/>
       <c r="BH57" s="2"/>
     </row>
-    <row r="58" spans="1:60">
+    <row r="58" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -4150,7 +4180,7 @@
       <c r="BG58" s="2"/>
       <c r="BH58" s="2"/>
     </row>
-    <row r="59" spans="1:60">
+    <row r="59" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -4212,7 +4242,7 @@
       <c r="BG59" s="2"/>
       <c r="BH59" s="2"/>
     </row>
-    <row r="60" spans="1:60">
+    <row r="60" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -4274,7 +4304,7 @@
       <c r="BG60" s="2"/>
       <c r="BH60" s="2"/>
     </row>
-    <row r="61" spans="1:60">
+    <row r="61" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -4336,7 +4366,7 @@
       <c r="BG61" s="2"/>
       <c r="BH61" s="2"/>
     </row>
-    <row r="62" spans="1:60">
+    <row r="62" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -4398,7 +4428,7 @@
       <c r="BG62" s="2"/>
       <c r="BH62" s="2"/>
     </row>
-    <row r="63" spans="1:60">
+    <row r="63" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -4460,7 +4490,7 @@
       <c r="BG63" s="2"/>
       <c r="BH63" s="2"/>
     </row>
-    <row r="64" spans="1:60">
+    <row r="64" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -4522,7 +4552,7 @@
       <c r="BG64" s="2"/>
       <c r="BH64" s="2"/>
     </row>
-    <row r="65" spans="1:60">
+    <row r="65" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -4584,7 +4614,7 @@
       <c r="BG65" s="2"/>
       <c r="BH65" s="2"/>
     </row>
-    <row r="66" spans="1:60">
+    <row r="66" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -4646,7 +4676,7 @@
       <c r="BG66" s="2"/>
       <c r="BH66" s="2"/>
     </row>
-    <row r="67" spans="1:60">
+    <row r="67" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -4708,7 +4738,7 @@
       <c r="BG67" s="2"/>
       <c r="BH67" s="2"/>
     </row>
-    <row r="68" spans="1:60">
+    <row r="68" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -4770,7 +4800,7 @@
       <c r="BG68" s="2"/>
       <c r="BH68" s="2"/>
     </row>
-    <row r="69" spans="1:60">
+    <row r="69" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -4832,7 +4862,7 @@
       <c r="BG69" s="2"/>
       <c r="BH69" s="2"/>
     </row>
-    <row r="70" spans="1:60">
+    <row r="70" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -4894,7 +4924,7 @@
       <c r="BG70" s="2"/>
       <c r="BH70" s="2"/>
     </row>
-    <row r="71" spans="1:60">
+    <row r="71" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4956,7 +4986,7 @@
       <c r="BG71" s="2"/>
       <c r="BH71" s="2"/>
     </row>
-    <row r="72" spans="1:60">
+    <row r="72" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -5018,7 +5048,7 @@
       <c r="BG72" s="2"/>
       <c r="BH72" s="2"/>
     </row>
-    <row r="73" spans="1:60">
+    <row r="73" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -5080,7 +5110,7 @@
       <c r="BG73" s="2"/>
       <c r="BH73" s="2"/>
     </row>
-    <row r="74" spans="1:60">
+    <row r="74" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -5142,7 +5172,7 @@
       <c r="BG74" s="2"/>
       <c r="BH74" s="2"/>
     </row>
-    <row r="75" spans="1:60">
+    <row r="75" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -5204,7 +5234,7 @@
       <c r="BG75" s="2"/>
       <c r="BH75" s="2"/>
     </row>
-    <row r="76" spans="1:60">
+    <row r="76" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -5266,7 +5296,7 @@
       <c r="BG76" s="2"/>
       <c r="BH76" s="2"/>
     </row>
-    <row r="77" spans="1:60">
+    <row r="77" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -5328,7 +5358,7 @@
       <c r="BG77" s="2"/>
       <c r="BH77" s="2"/>
     </row>
-    <row r="78" spans="1:60">
+    <row r="78" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -5390,7 +5420,7 @@
       <c r="BG78" s="2"/>
       <c r="BH78" s="2"/>
     </row>
-    <row r="79" spans="1:60">
+    <row r="79" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -5452,7 +5482,7 @@
       <c r="BG79" s="2"/>
       <c r="BH79" s="2"/>
     </row>
-    <row r="80" spans="1:60">
+    <row r="80" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -5514,7 +5544,7 @@
       <c r="BG80" s="2"/>
       <c r="BH80" s="2"/>
     </row>
-    <row r="81" spans="1:60">
+    <row r="81" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -5576,7 +5606,7 @@
       <c r="BG81" s="2"/>
       <c r="BH81" s="2"/>
     </row>
-    <row r="82" spans="1:60">
+    <row r="82" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -5638,7 +5668,7 @@
       <c r="BG82" s="2"/>
       <c r="BH82" s="2"/>
     </row>
-    <row r="83" spans="1:60">
+    <row r="83" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -5700,7 +5730,7 @@
       <c r="BG83" s="2"/>
       <c r="BH83" s="2"/>
     </row>
-    <row r="84" spans="1:60">
+    <row r="84" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -5762,7 +5792,7 @@
       <c r="BG84" s="2"/>
       <c r="BH84" s="2"/>
     </row>
-    <row r="85" spans="1:60">
+    <row r="85" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -5824,7 +5854,7 @@
       <c r="BG85" s="2"/>
       <c r="BH85" s="2"/>
     </row>
-    <row r="86" spans="1:60">
+    <row r="86" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -5886,7 +5916,7 @@
       <c r="BG86" s="2"/>
       <c r="BH86" s="2"/>
     </row>
-    <row r="87" spans="1:60">
+    <row r="87" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -5948,7 +5978,7 @@
       <c r="BG87" s="2"/>
       <c r="BH87" s="2"/>
     </row>
-    <row r="88" spans="1:60">
+    <row r="88" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -6010,7 +6040,7 @@
       <c r="BG88" s="2"/>
       <c r="BH88" s="2"/>
     </row>
-    <row r="89" spans="1:60">
+    <row r="89" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -6072,7 +6102,7 @@
       <c r="BG89" s="2"/>
       <c r="BH89" s="2"/>
     </row>
-    <row r="90" spans="1:60">
+    <row r="90" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -6134,7 +6164,7 @@
       <c r="BG90" s="2"/>
       <c r="BH90" s="2"/>
     </row>
-    <row r="91" spans="1:60">
+    <row r="91" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -6196,7 +6226,7 @@
       <c r="BG91" s="2"/>
       <c r="BH91" s="2"/>
     </row>
-    <row r="92" spans="1:60">
+    <row r="92" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -6258,7 +6288,7 @@
       <c r="BG92" s="2"/>
       <c r="BH92" s="2"/>
     </row>
-    <row r="93" spans="1:60">
+    <row r="93" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -6320,7 +6350,7 @@
       <c r="BG93" s="2"/>
       <c r="BH93" s="2"/>
     </row>
-    <row r="94" spans="1:60">
+    <row r="94" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -6382,7 +6412,7 @@
       <c r="BG94" s="2"/>
       <c r="BH94" s="2"/>
     </row>
-    <row r="95" spans="1:60">
+    <row r="95" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -6444,7 +6474,7 @@
       <c r="BG95" s="2"/>
       <c r="BH95" s="2"/>
     </row>
-    <row r="96" spans="1:60">
+    <row r="96" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -6506,7 +6536,7 @@
       <c r="BG96" s="2"/>
       <c r="BH96" s="2"/>
     </row>
-    <row r="97" spans="1:60">
+    <row r="97" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -6568,7 +6598,7 @@
       <c r="BG97" s="2"/>
       <c r="BH97" s="2"/>
     </row>
-    <row r="98" spans="1:60">
+    <row r="98" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -6630,7 +6660,7 @@
       <c r="BG98" s="2"/>
       <c r="BH98" s="2"/>
     </row>
-    <row r="99" spans="1:60">
+    <row r="99" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -6692,7 +6722,7 @@
       <c r="BG99" s="2"/>
       <c r="BH99" s="2"/>
     </row>
-    <row r="100" spans="1:60">
+    <row r="100" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -6754,7 +6784,7 @@
       <c r="BG100" s="2"/>
       <c r="BH100" s="2"/>
     </row>
-    <row r="101" spans="1:60">
+    <row r="101" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -6816,7 +6846,7 @@
       <c r="BG101" s="2"/>
       <c r="BH101" s="2"/>
     </row>
-    <row r="102" spans="1:60">
+    <row r="102" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -6878,7 +6908,7 @@
       <c r="BG102" s="2"/>
       <c r="BH102" s="2"/>
     </row>
-    <row r="103" spans="1:60">
+    <row r="103" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -6940,7 +6970,7 @@
       <c r="BG103" s="2"/>
       <c r="BH103" s="2"/>
     </row>
-    <row r="104" spans="1:60">
+    <row r="104" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -7002,7 +7032,7 @@
       <c r="BG104" s="2"/>
       <c r="BH104" s="2"/>
     </row>
-    <row r="105" spans="1:60">
+    <row r="105" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -7064,7 +7094,7 @@
       <c r="BG105" s="2"/>
       <c r="BH105" s="2"/>
     </row>
-    <row r="106" spans="1:60">
+    <row r="106" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -7126,7 +7156,7 @@
       <c r="BG106" s="2"/>
       <c r="BH106" s="2"/>
     </row>
-    <row r="107" spans="1:60">
+    <row r="107" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -7188,7 +7218,7 @@
       <c r="BG107" s="2"/>
       <c r="BH107" s="2"/>
     </row>
-    <row r="108" spans="1:60">
+    <row r="108" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -7250,7 +7280,7 @@
       <c r="BG108" s="2"/>
       <c r="BH108" s="2"/>
     </row>
-    <row r="109" spans="1:60">
+    <row r="109" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -7312,7 +7342,7 @@
       <c r="BG109" s="2"/>
       <c r="BH109" s="2"/>
     </row>
-    <row r="110" spans="1:60">
+    <row r="110" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -7374,7 +7404,7 @@
       <c r="BG110" s="2"/>
       <c r="BH110" s="2"/>
     </row>
-    <row r="111" spans="1:60">
+    <row r="111" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -7436,7 +7466,7 @@
       <c r="BG111" s="2"/>
       <c r="BH111" s="2"/>
     </row>
-    <row r="112" spans="1:60">
+    <row r="112" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -7498,7 +7528,7 @@
       <c r="BG112" s="2"/>
       <c r="BH112" s="2"/>
     </row>
-    <row r="113" spans="1:60">
+    <row r="113" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -7560,7 +7590,7 @@
       <c r="BG113" s="2"/>
       <c r="BH113" s="2"/>
     </row>
-    <row r="114" spans="1:60">
+    <row r="114" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -7622,7 +7652,7 @@
       <c r="BG114" s="2"/>
       <c r="BH114" s="2"/>
     </row>
-    <row r="115" spans="1:60">
+    <row r="115" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -7684,7 +7714,7 @@
       <c r="BG115" s="2"/>
       <c r="BH115" s="2"/>
     </row>
-    <row r="116" spans="1:60">
+    <row r="116" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -7746,7 +7776,7 @@
       <c r="BG116" s="2"/>
       <c r="BH116" s="2"/>
     </row>
-    <row r="117" spans="1:60">
+    <row r="117" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -7808,7 +7838,7 @@
       <c r="BG117" s="2"/>
       <c r="BH117" s="2"/>
     </row>
-    <row r="118" spans="1:60">
+    <row r="118" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -7870,7 +7900,7 @@
       <c r="BG118" s="2"/>
       <c r="BH118" s="2"/>
     </row>
-    <row r="119" spans="1:60">
+    <row r="119" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -7932,7 +7962,7 @@
       <c r="BG119" s="2"/>
       <c r="BH119" s="2"/>
     </row>
-    <row r="120" spans="1:60">
+    <row r="120" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -7994,7 +8024,7 @@
       <c r="BG120" s="2"/>
       <c r="BH120" s="2"/>
     </row>
-    <row r="121" spans="1:60">
+    <row r="121" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -8056,7 +8086,7 @@
       <c r="BG121" s="2"/>
       <c r="BH121" s="2"/>
     </row>
-    <row r="122" spans="1:60">
+    <row r="122" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -8118,7 +8148,7 @@
       <c r="BG122" s="2"/>
       <c r="BH122" s="2"/>
     </row>
-    <row r="123" spans="1:60">
+    <row r="123" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -8180,7 +8210,7 @@
       <c r="BG123" s="2"/>
       <c r="BH123" s="2"/>
     </row>
-    <row r="124" spans="1:60">
+    <row r="124" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -8242,7 +8272,7 @@
       <c r="BG124" s="2"/>
       <c r="BH124" s="2"/>
     </row>
-    <row r="125" spans="1:60">
+    <row r="125" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -8304,7 +8334,7 @@
       <c r="BG125" s="2"/>
       <c r="BH125" s="2"/>
     </row>
-    <row r="126" spans="1:60">
+    <row r="126" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -8366,7 +8396,7 @@
       <c r="BG126" s="2"/>
       <c r="BH126" s="2"/>
     </row>
-    <row r="127" spans="1:60">
+    <row r="127" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -8428,7 +8458,7 @@
       <c r="BG127" s="2"/>
       <c r="BH127" s="2"/>
     </row>
-    <row r="128" spans="1:60">
+    <row r="128" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -8490,7 +8520,7 @@
       <c r="BG128" s="2"/>
       <c r="BH128" s="2"/>
     </row>
-    <row r="129" spans="1:60">
+    <row r="129" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -8552,7 +8582,7 @@
       <c r="BG129" s="2"/>
       <c r="BH129" s="2"/>
     </row>
-    <row r="130" spans="1:60">
+    <row r="130" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -8614,7 +8644,7 @@
       <c r="BG130" s="2"/>
       <c r="BH130" s="2"/>
     </row>
-    <row r="131" spans="1:60">
+    <row r="131" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -8676,7 +8706,7 @@
       <c r="BG131" s="2"/>
       <c r="BH131" s="2"/>
     </row>
-    <row r="132" spans="1:60">
+    <row r="132" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -8738,7 +8768,7 @@
       <c r="BG132" s="2"/>
       <c r="BH132" s="2"/>
     </row>
-    <row r="133" spans="1:60">
+    <row r="133" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -8800,7 +8830,7 @@
       <c r="BG133" s="2"/>
       <c r="BH133" s="2"/>
     </row>
-    <row r="134" spans="1:60">
+    <row r="134" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -8862,7 +8892,7 @@
       <c r="BG134" s="2"/>
       <c r="BH134" s="2"/>
     </row>
-    <row r="135" spans="1:60">
+    <row r="135" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -8924,7 +8954,7 @@
       <c r="BG135" s="2"/>
       <c r="BH135" s="2"/>
     </row>
-    <row r="136" spans="1:60">
+    <row r="136" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -8986,7 +9016,7 @@
       <c r="BG136" s="2"/>
       <c r="BH136" s="2"/>
     </row>
-    <row r="137" spans="1:60">
+    <row r="137" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -9048,7 +9078,7 @@
       <c r="BG137" s="2"/>
       <c r="BH137" s="2"/>
     </row>
-    <row r="138" spans="1:60">
+    <row r="138" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -9110,7 +9140,7 @@
       <c r="BG138" s="2"/>
       <c r="BH138" s="2"/>
     </row>
-    <row r="139" spans="1:60">
+    <row r="139" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -9172,7 +9202,7 @@
       <c r="BG139" s="2"/>
       <c r="BH139" s="2"/>
     </row>
-    <row r="140" spans="1:60">
+    <row r="140" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -9234,7 +9264,7 @@
       <c r="BG140" s="2"/>
       <c r="BH140" s="2"/>
     </row>
-    <row r="141" spans="1:60">
+    <row r="141" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -9296,7 +9326,7 @@
       <c r="BG141" s="2"/>
       <c r="BH141" s="2"/>
     </row>
-    <row r="142" spans="1:60">
+    <row r="142" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -9358,7 +9388,7 @@
       <c r="BG142" s="2"/>
       <c r="BH142" s="2"/>
     </row>
-    <row r="143" spans="1:60">
+    <row r="143" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -9420,7 +9450,7 @@
       <c r="BG143" s="2"/>
       <c r="BH143" s="2"/>
     </row>
-    <row r="144" spans="1:60">
+    <row r="144" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -9482,7 +9512,7 @@
       <c r="BG144" s="2"/>
       <c r="BH144" s="2"/>
     </row>
-    <row r="145" spans="1:60">
+    <row r="145" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -9544,7 +9574,7 @@
       <c r="BG145" s="2"/>
       <c r="BH145" s="2"/>
     </row>
-    <row r="146" spans="1:60">
+    <row r="146" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -9606,7 +9636,7 @@
       <c r="BG146" s="2"/>
       <c r="BH146" s="2"/>
     </row>
-    <row r="147" spans="1:60">
+    <row r="147" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -9668,7 +9698,7 @@
       <c r="BG147" s="2"/>
       <c r="BH147" s="2"/>
     </row>
-    <row r="148" spans="1:60">
+    <row r="148" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -9730,7 +9760,7 @@
       <c r="BG148" s="2"/>
       <c r="BH148" s="2"/>
     </row>
-    <row r="149" spans="1:60">
+    <row r="149" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -9792,7 +9822,7 @@
       <c r="BG149" s="2"/>
       <c r="BH149" s="2"/>
     </row>
-    <row r="150" spans="1:60">
+    <row r="150" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -9854,7 +9884,7 @@
       <c r="BG150" s="2"/>
       <c r="BH150" s="2"/>
     </row>
-    <row r="151" spans="1:60">
+    <row r="151" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -9916,7 +9946,7 @@
       <c r="BG151" s="2"/>
       <c r="BH151" s="2"/>
     </row>
-    <row r="152" spans="1:60">
+    <row r="152" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -9978,7 +10008,7 @@
       <c r="BG152" s="2"/>
       <c r="BH152" s="2"/>
     </row>
-    <row r="153" spans="1:60">
+    <row r="153" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -10040,7 +10070,7 @@
       <c r="BG153" s="2"/>
       <c r="BH153" s="2"/>
     </row>
-    <row r="154" spans="1:60">
+    <row r="154" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -10102,7 +10132,7 @@
       <c r="BG154" s="2"/>
       <c r="BH154" s="2"/>
     </row>
-    <row r="155" spans="1:60">
+    <row r="155" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -10164,7 +10194,7 @@
       <c r="BG155" s="2"/>
       <c r="BH155" s="2"/>
     </row>
-    <row r="156" spans="1:60">
+    <row r="156" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -10226,7 +10256,7 @@
       <c r="BG156" s="2"/>
       <c r="BH156" s="2"/>
     </row>
-    <row r="157" spans="1:60">
+    <row r="157" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -10288,7 +10318,7 @@
       <c r="BG157" s="2"/>
       <c r="BH157" s="2"/>
     </row>
-    <row r="158" spans="1:60">
+    <row r="158" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -10350,7 +10380,7 @@
       <c r="BG158" s="2"/>
       <c r="BH158" s="2"/>
     </row>
-    <row r="159" spans="1:60">
+    <row r="159" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -10412,7 +10442,7 @@
       <c r="BG159" s="2"/>
       <c r="BH159" s="2"/>
     </row>
-    <row r="160" spans="1:60">
+    <row r="160" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -10474,7 +10504,7 @@
       <c r="BG160" s="2"/>
       <c r="BH160" s="2"/>
     </row>
-    <row r="161" spans="1:60">
+    <row r="161" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -10536,7 +10566,7 @@
       <c r="BG161" s="2"/>
       <c r="BH161" s="2"/>
     </row>
-    <row r="162" spans="1:60">
+    <row r="162" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -10598,7 +10628,7 @@
       <c r="BG162" s="2"/>
       <c r="BH162" s="2"/>
     </row>
-    <row r="163" spans="1:60">
+    <row r="163" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -10660,7 +10690,7 @@
       <c r="BG163" s="2"/>
       <c r="BH163" s="2"/>
     </row>
-    <row r="164" spans="1:60">
+    <row r="164" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -10722,7 +10752,7 @@
       <c r="BG164" s="2"/>
       <c r="BH164" s="2"/>
     </row>
-    <row r="165" spans="1:60">
+    <row r="165" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -10784,7 +10814,7 @@
       <c r="BG165" s="2"/>
       <c r="BH165" s="2"/>
     </row>
-    <row r="166" spans="1:60">
+    <row r="166" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -10846,7 +10876,7 @@
       <c r="BG166" s="2"/>
       <c r="BH166" s="2"/>
     </row>
-    <row r="167" spans="1:60">
+    <row r="167" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -10908,7 +10938,7 @@
       <c r="BG167" s="2"/>
       <c r="BH167" s="2"/>
     </row>
-    <row r="168" spans="1:60">
+    <row r="168" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -10970,7 +11000,7 @@
       <c r="BG168" s="2"/>
       <c r="BH168" s="2"/>
     </row>
-    <row r="169" spans="1:60">
+    <row r="169" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -11032,7 +11062,7 @@
       <c r="BG169" s="2"/>
       <c r="BH169" s="2"/>
     </row>
-    <row r="170" spans="1:60">
+    <row r="170" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -11094,7 +11124,7 @@
       <c r="BG170" s="2"/>
       <c r="BH170" s="2"/>
     </row>
-    <row r="171" spans="1:60">
+    <row r="171" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -11156,7 +11186,7 @@
       <c r="BG171" s="2"/>
       <c r="BH171" s="2"/>
     </row>
-    <row r="172" spans="1:60">
+    <row r="172" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -11218,7 +11248,7 @@
       <c r="BG172" s="2"/>
       <c r="BH172" s="2"/>
     </row>
-    <row r="173" spans="1:60">
+    <row r="173" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -11280,7 +11310,7 @@
       <c r="BG173" s="2"/>
       <c r="BH173" s="2"/>
     </row>
-    <row r="174" spans="1:60">
+    <row r="174" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -11342,7 +11372,7 @@
       <c r="BG174" s="2"/>
       <c r="BH174" s="2"/>
     </row>
-    <row r="175" spans="1:60">
+    <row r="175" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -11404,7 +11434,7 @@
       <c r="BG175" s="2"/>
       <c r="BH175" s="2"/>
     </row>
-    <row r="176" spans="1:60">
+    <row r="176" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -11466,7 +11496,7 @@
       <c r="BG176" s="2"/>
       <c r="BH176" s="2"/>
     </row>
-    <row r="177" spans="1:60">
+    <row r="177" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -11528,7 +11558,7 @@
       <c r="BG177" s="2"/>
       <c r="BH177" s="2"/>
     </row>
-    <row r="178" spans="1:60">
+    <row r="178" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -11590,7 +11620,7 @@
       <c r="BG178" s="2"/>
       <c r="BH178" s="2"/>
     </row>
-    <row r="179" spans="1:60">
+    <row r="179" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -11652,7 +11682,7 @@
       <c r="BG179" s="2"/>
       <c r="BH179" s="2"/>
     </row>
-    <row r="180" spans="1:60">
+    <row r="180" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -11714,7 +11744,7 @@
       <c r="BG180" s="2"/>
       <c r="BH180" s="2"/>
     </row>
-    <row r="181" spans="1:60">
+    <row r="181" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -11776,7 +11806,7 @@
       <c r="BG181" s="2"/>
       <c r="BH181" s="2"/>
     </row>
-    <row r="182" spans="1:60">
+    <row r="182" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -11838,7 +11868,7 @@
       <c r="BG182" s="2"/>
       <c r="BH182" s="2"/>
     </row>
-    <row r="183" spans="1:60">
+    <row r="183" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -11900,7 +11930,7 @@
       <c r="BG183" s="2"/>
       <c r="BH183" s="2"/>
     </row>
-    <row r="184" spans="1:60">
+    <row r="184" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -11962,7 +11992,7 @@
       <c r="BG184" s="2"/>
       <c r="BH184" s="2"/>
     </row>
-    <row r="185" spans="1:60">
+    <row r="185" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -12026,6 +12056,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AP25:AW25"/>
+    <mergeCell ref="AX25:BE25"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="J25:Q25"/>
+    <mergeCell ref="R25:Y25"/>
+    <mergeCell ref="Z25:AG25"/>
+    <mergeCell ref="AH25:AO25"/>
+    <mergeCell ref="BF2:BM2"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="J2:Q2"/>
+    <mergeCell ref="R2:Y2"/>
+    <mergeCell ref="Z2:AG2"/>
+    <mergeCell ref="AH2:AO2"/>
     <mergeCell ref="Z13:AG13"/>
     <mergeCell ref="AH13:AO13"/>
     <mergeCell ref="AP13:AW13"/>
@@ -12037,19 +12080,6 @@
     <mergeCell ref="R13:Y13"/>
     <mergeCell ref="AP2:AW2"/>
     <mergeCell ref="AX2:BE2"/>
-    <mergeCell ref="BF2:BM2"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="R2:Y2"/>
-    <mergeCell ref="Z2:AG2"/>
-    <mergeCell ref="AH2:AO2"/>
-    <mergeCell ref="AP25:AW25"/>
-    <mergeCell ref="AX25:BE25"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="J25:Q25"/>
-    <mergeCell ref="R25:Y25"/>
-    <mergeCell ref="Z25:AG25"/>
-    <mergeCell ref="AH25:AO25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -12067,7 +12097,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
@@ -12084,7 +12114,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>